<commit_message>
Update external data files w/ new taxonomy
</commit_message>
<xml_diff>
--- a/ExternalData/masterColors.xlsx
+++ b/ExternalData/masterColors.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1560" windowWidth="23040" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="-28460" yWindow="-1980" windowWidth="23040" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
     <sheet name="Tribes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tribes!#REF!</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="1">Tribes!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tribes!$G$1:$J$32</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="1">Tribes!$L$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="102">
   <si>
     <t>Short name</t>
   </si>
@@ -281,27 +281,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>acTH1</t>
-  </si>
-  <si>
-    <t>acTH1-A</t>
-  </si>
-  <si>
-    <t>acTH1-A1</t>
-  </si>
-  <si>
-    <t>Luna1-A4</t>
-  </si>
-  <si>
-    <t>acSTL</t>
-  </si>
-  <si>
-    <t>acSTL-A</t>
-  </si>
-  <si>
-    <t>acSTL-A1</t>
-  </si>
-  <si>
     <t>acIB-AMD-6</t>
   </si>
   <si>
@@ -336,9 +315,6 @@
   </si>
   <si>
     <t>Rhodoluna</t>
-  </si>
-  <si>
-    <t>w</t>
   </si>
   <si>
     <t>y</t>
@@ -418,8 +394,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -466,11 +466,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -488,6 +486,18 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -505,6 +515,18 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -834,19 +856,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18">
+    <row r="1" spans="1:16" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,14 +885,15 @@
       <c r="E1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="17">
-      <c r="A2" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" ht="18" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -878,19 +902,15 @@
       <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="17">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -899,145 +919,117 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="17">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="17">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="17">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="17">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="17">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="17">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="9" spans="1:16" ht="17" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="17">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1046,19 +1038,15 @@
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="17">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1067,40 +1055,32 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="17">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" ht="17">
-      <c r="A13" s="2" t="s">
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1109,61 +1089,49 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" ht="17">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" ht="17">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E15" s="2">
         <v>0.75</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="17">
-      <c r="A16" s="2" t="s">
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1172,19 +1140,15 @@
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" ht="17">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1193,19 +1157,15 @@
       <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" ht="17">
-      <c r="A18" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1214,40 +1174,32 @@
       <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" ht="17">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" ht="17">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1256,19 +1208,15 @@
       <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" ht="17">
-      <c r="A21" s="2" t="s">
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1277,19 +1225,15 @@
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" ht="17">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1298,41 +1242,33 @@
       <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" ht="17">
-      <c r="A23" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" ht="17">
-      <c r="A24" s="3" t="s">
-        <v>93</v>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>5</v>
@@ -1340,145 +1276,117 @@
       <c r="C24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" ht="17">
-      <c r="A25" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="3" t="s">
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" ht="17">
-      <c r="A26" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="1:11" ht="17">
-      <c r="A27" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="3" t="s">
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" ht="17">
-      <c r="A28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="3" t="s">
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" ht="17">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" ht="17">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>102</v>
+      <c r="D30" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H30" s="4"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="1:11" ht="17">
-      <c r="A31" s="2" t="s">
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1487,61 +1395,49 @@
       <c r="C31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E31" s="2">
         <v>0.25</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" ht="17">
-      <c r="A32" s="2" t="s">
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" ht="17">
-      <c r="A33" s="2" t="s">
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" ht="17">
-      <c r="A34" s="2" t="s">
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1550,61 +1446,49 @@
       <c r="C34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" ht="17">
-      <c r="A35" s="2" t="s">
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" ht="17">
-      <c r="A36" s="2" t="s">
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" ht="17">
-      <c r="A37" s="2" t="s">
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1613,19 +1497,15 @@
       <c r="C37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" ht="17">
-      <c r="A38" s="2" t="s">
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1634,61 +1514,49 @@
       <c r="C38" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" ht="17">
-      <c r="A39" s="2" t="s">
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" ht="17">
-      <c r="A40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" ht="17">
-      <c r="A41" s="2" t="s">
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1697,19 +1565,15 @@
       <c r="C41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" ht="17">
-      <c r="A42" s="2" t="s">
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1718,40 +1582,32 @@
       <c r="C42" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" ht="17">
-      <c r="A43" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" ht="17">
-      <c r="A44" s="2" t="s">
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1760,19 +1616,15 @@
       <c r="C44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" ht="17">
-      <c r="A45" s="2" t="s">
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1781,19 +1633,15 @@
       <c r="C45" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" ht="17">
-      <c r="A46" s="2" t="s">
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1802,124 +1650,100 @@
       <c r="C46" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" ht="17">
-      <c r="A47" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B47" s="3" t="s">
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E47" s="2">
         <v>0.75</v>
       </c>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" ht="17">
-      <c r="A48" s="2" t="s">
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-    </row>
-    <row r="49" spans="1:11" ht="17">
-      <c r="A49" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="2" t="s">
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" ht="17">
-      <c r="A50" s="2" t="s">
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="B50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-    </row>
-    <row r="51" spans="1:11" ht="17">
-      <c r="A51" s="2" t="s">
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-    </row>
-    <row r="52" spans="1:11" ht="17">
-      <c r="A52" s="2" t="s">
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -1928,40 +1752,32 @@
       <c r="C52" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-    </row>
-    <row r="53" spans="1:11" ht="17">
-      <c r="A53" s="2" t="s">
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" ht="17">
-      <c r="A54" s="2" t="s">
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -1970,40 +1786,32 @@
       <c r="C54" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-    </row>
-    <row r="55" spans="1:11" ht="17">
-      <c r="A55" s="2" t="s">
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-    </row>
-    <row r="56" spans="1:11" ht="17">
-      <c r="A56" s="2" t="s">
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2012,82 +1820,66 @@
       <c r="C56" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-    </row>
-    <row r="57" spans="1:11" ht="17">
-      <c r="A57" s="2" t="s">
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="B57" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-    </row>
-    <row r="58" spans="1:11" ht="17">
-      <c r="A58" s="2" t="s">
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H58" s="2"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-    </row>
-    <row r="59" spans="1:11" ht="17">
-      <c r="A59" s="2" t="s">
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-    </row>
-    <row r="60" spans="1:11" ht="17">
-      <c r="A60" s="2" t="s">
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -2096,41 +1888,33 @@
       <c r="C60" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-    </row>
-    <row r="61" spans="1:11" ht="17">
-      <c r="A61" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B61" s="3" t="s">
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-    </row>
-    <row r="62" spans="1:11" ht="17">
-      <c r="A62" s="2" t="s">
-        <v>109</v>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>5</v>
@@ -2138,19 +1922,15 @@
       <c r="C62" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-    </row>
-    <row r="63" spans="1:11" ht="17">
-      <c r="A63" s="2" t="s">
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -2159,95 +1939,87 @@
       <c r="C63" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-    </row>
-    <row r="64" spans="1:11" ht="17">
-      <c r="A64" s="2" t="s">
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" ht="17">
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" ht="17">
+    <row r="66" spans="1:5">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" ht="17">
+    <row r="67" spans="1:5">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5" ht="17">
+    <row r="68" spans="1:5">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" ht="17">
+    <row r="69" spans="1:5">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:5" ht="17">
+    <row r="70" spans="1:5">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" ht="17">
+    <row r="71" spans="1:5">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" ht="17">
+    <row r="72" spans="1:5">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5" ht="17">
+    <row r="73" spans="1:5">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -2255,7 +2027,7 @@
       <c r="E73" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F64">
+  <sortState ref="A2:E64">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2270,13 +2042,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2289,8 +2061,16 @@
       <c r="D1" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" ht="17" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2303,8 +2083,14 @@
       <c r="D2" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" ht="17">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2317,8 +2103,14 @@
       <c r="D3" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="17">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -2331,8 +2123,14 @@
       <c r="D4" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="17">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2345,8 +2143,14 @@
       <c r="D5" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" ht="17">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2359,8 +2163,14 @@
       <c r="D6" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" ht="17">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2368,13 +2178,19 @@
         <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="17">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" ht="17" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -2387,120 +2203,224 @@
       <c r="D8" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17">
-      <c r="A9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>91</v>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="18" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17">
+        <v>83</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" ht="17">
       <c r="A10" s="3" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17">
+        <v>83</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" ht="17">
       <c r="A11" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="17">
-      <c r="A12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" ht="17">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" ht="18" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17">
-      <c r="A14" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D13" s="2">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="17">
-      <c r="A15" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17">
-      <c r="A16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" ht="17">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" ht="17">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="17">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="7:10" ht="17">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="7:10" ht="17">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="7:10" ht="17">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="7:10" ht="17">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="7:10" ht="17">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="7:10" ht="17">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="7:10" ht="17">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="7:10" ht="17">
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="7:10" ht="17">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="7:10" ht="17">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="7:10" ht="17">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="7:10" ht="17">
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="7:10" ht="17">
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="7:10" ht="17">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="7:10" ht="18">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="7:10" ht="17">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="7:10" ht="17">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="63" ht="17" customHeight="1"/>
   </sheetData>
+  <sortState ref="A2:D14">
+    <sortCondition ref="A2:A14"/>
+    <sortCondition ref="B2:B14"/>
+    <sortCondition ref="C2:C14"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>